<commit_message>
git: problem 1 data
</commit_message>
<xml_diff>
--- a/Table for heuristics analysis.xlsx
+++ b/Table for heuristics analysis.xlsx
@@ -674,8 +674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D3:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -724,98 +724,174 @@
       <c r="F6" s="9">
         <v>43</v>
       </c>
-      <c r="G6" s="10"/>
-      <c r="H6" s="11"/>
+      <c r="G6" s="10">
+        <v>56</v>
+      </c>
+      <c r="H6" s="11">
+        <v>180</v>
+      </c>
       <c r="I6" s="12"/>
     </row>
     <row r="7" spans="4:9" ht="15" x14ac:dyDescent="0.25">
       <c r="D7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="14"/>
+      <c r="E7" s="13">
+        <v>2.605</v>
+      </c>
+      <c r="F7" s="13">
+        <v>1458</v>
+      </c>
+      <c r="G7" s="13">
+        <v>1459</v>
+      </c>
+      <c r="H7" s="14">
+        <v>5960</v>
+      </c>
       <c r="I7" s="15"/>
     </row>
     <row r="8" spans="4:9" ht="15" x14ac:dyDescent="0.25">
       <c r="D8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="14"/>
+      <c r="E8" s="13">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="F8" s="13">
+        <v>21</v>
+      </c>
+      <c r="G8" s="13">
+        <v>22</v>
+      </c>
+      <c r="H8" s="14">
+        <v>84</v>
+      </c>
       <c r="I8" s="15"/>
     </row>
     <row r="9" spans="4:9" ht="15" x14ac:dyDescent="0.25">
       <c r="D9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="14"/>
+      <c r="E9" s="13">
+        <v>0.19900000000000001</v>
+      </c>
+      <c r="F9" s="13">
+        <v>101</v>
+      </c>
+      <c r="G9" s="13">
+        <v>271</v>
+      </c>
+      <c r="H9" s="14">
+        <v>414</v>
+      </c>
       <c r="I9" s="15"/>
     </row>
     <row r="10" spans="4:9" ht="15" x14ac:dyDescent="0.25">
       <c r="D10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="14"/>
+      <c r="E10" s="13">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="F10" s="13">
+        <v>55</v>
+      </c>
+      <c r="G10" s="13">
+        <v>57</v>
+      </c>
+      <c r="H10" s="14">
+        <v>224</v>
+      </c>
       <c r="I10" s="15"/>
     </row>
     <row r="11" spans="4:9" ht="15" x14ac:dyDescent="0.25">
       <c r="D11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="14"/>
+      <c r="E11" s="13">
+        <v>5.23</v>
+      </c>
+      <c r="F11" s="13">
+        <v>4229</v>
+      </c>
+      <c r="G11" s="13">
+        <v>4230</v>
+      </c>
+      <c r="H11" s="14">
+        <v>17023</v>
+      </c>
       <c r="I11" s="15"/>
     </row>
     <row r="12" spans="4:9" ht="15" x14ac:dyDescent="0.25">
       <c r="D12" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="14"/>
+      <c r="E12" s="13">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="F12" s="13">
+        <v>7</v>
+      </c>
+      <c r="G12" s="13">
+        <v>9</v>
+      </c>
+      <c r="H12" s="14">
+        <v>28</v>
+      </c>
       <c r="I12" s="15"/>
     </row>
     <row r="13" spans="4:9" ht="15" x14ac:dyDescent="0.25">
       <c r="D13" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="14"/>
+      <c r="E13" s="13">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="F13" s="13">
+        <v>55</v>
+      </c>
+      <c r="G13" s="13">
+        <v>57</v>
+      </c>
+      <c r="H13" s="14">
+        <v>224</v>
+      </c>
       <c r="I13" s="15"/>
     </row>
     <row r="14" spans="4:9" ht="15" x14ac:dyDescent="0.25">
       <c r="D14" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="14"/>
+      <c r="E14" s="13">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="F14" s="13">
+        <v>41</v>
+      </c>
+      <c r="G14" s="13">
+        <v>43</v>
+      </c>
+      <c r="H14" s="14">
+        <v>170</v>
+      </c>
       <c r="I14" s="15"/>
     </row>
     <row r="15" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D15" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="19"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="17"/>
+      <c r="E15" s="19">
+        <v>0.874</v>
+      </c>
+      <c r="F15" s="16">
+        <v>11</v>
+      </c>
+      <c r="G15" s="16">
+        <v>13</v>
+      </c>
+      <c r="H15" s="17">
+        <v>50</v>
+      </c>
       <c r="I15" s="18"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Problem 2 data
</commit_message>
<xml_diff>
--- a/Table for heuristics analysis.xlsx
+++ b/Table for heuristics analysis.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="23">
   <si>
     <t>Solving Air Cargo Problem 1</t>
   </si>
@@ -84,13 +84,22 @@
   </si>
   <si>
     <t>Path Length</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -109,14 +118,36 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF7C5D"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="19">
     <border>
@@ -384,7 +415,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -396,8 +427,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -434,13 +466,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF7C5D"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -717,8 +780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D3:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" topLeftCell="D12" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -737,26 +800,26 @@
       </c>
     </row>
     <row r="4" spans="4:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="I5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="21" t="s">
+      <c r="J5" s="20" t="s">
         <v>2</v>
       </c>
     </row>
@@ -764,211 +827,231 @@
       <c r="D6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="8">
         <v>0.13200000000000001</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="8">
         <v>6</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="8">
         <v>43</v>
       </c>
-      <c r="H6" s="10">
+      <c r="H6" s="9">
         <v>56</v>
       </c>
-      <c r="I6" s="11">
+      <c r="I6" s="10">
         <v>180</v>
       </c>
-      <c r="J6" s="12"/>
+      <c r="J6" s="11" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="7" spans="4:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="12">
         <v>2.605</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F7" s="12">
         <v>6</v>
       </c>
-      <c r="G7" s="13">
+      <c r="G7" s="12">
         <v>1458</v>
       </c>
-      <c r="H7" s="13">
+      <c r="H7" s="12">
         <v>1459</v>
       </c>
-      <c r="I7" s="14">
+      <c r="I7" s="13">
         <v>5960</v>
       </c>
-      <c r="J7" s="15"/>
+      <c r="J7" s="14" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="8" spans="4:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="12">
         <v>3.6999999999999998E-2</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F8" s="12">
         <v>20</v>
       </c>
-      <c r="G8" s="13">
+      <c r="G8" s="12">
         <v>21</v>
       </c>
-      <c r="H8" s="13">
-        <v>22</v>
-      </c>
-      <c r="I8" s="14">
+      <c r="H8" s="12">
+        <v>22</v>
+      </c>
+      <c r="I8" s="13">
         <v>84</v>
       </c>
-      <c r="J8" s="15"/>
+      <c r="J8" s="14" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="9" spans="4:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="12">
         <v>0.19900000000000001</v>
       </c>
-      <c r="F9" s="13">
+      <c r="F9" s="12">
         <v>50</v>
       </c>
-      <c r="G9" s="13">
+      <c r="G9" s="12">
         <v>101</v>
       </c>
-      <c r="H9" s="13">
+      <c r="H9" s="12">
         <v>271</v>
       </c>
-      <c r="I9" s="14">
+      <c r="I9" s="13">
         <v>414</v>
       </c>
-      <c r="J9" s="15"/>
+      <c r="J9" s="14" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="10" spans="4:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10" s="12">
         <v>9.1999999999999998E-2</v>
       </c>
-      <c r="F10" s="13">
+      <c r="F10" s="12">
         <v>6</v>
       </c>
-      <c r="G10" s="13">
+      <c r="G10" s="12">
         <v>55</v>
       </c>
-      <c r="H10" s="13">
+      <c r="H10" s="12">
         <v>57</v>
       </c>
-      <c r="I10" s="14">
+      <c r="I10" s="13">
         <v>224</v>
       </c>
-      <c r="J10" s="15"/>
+      <c r="J10" s="14" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="11" spans="4:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="13">
+      <c r="E11" s="12">
         <v>5.23</v>
       </c>
-      <c r="F11" s="13">
+      <c r="F11" s="12">
         <v>6</v>
       </c>
-      <c r="G11" s="13">
+      <c r="G11" s="12">
         <v>4229</v>
       </c>
-      <c r="H11" s="13">
+      <c r="H11" s="12">
         <v>4230</v>
       </c>
-      <c r="I11" s="14">
+      <c r="I11" s="13">
         <v>17023</v>
       </c>
-      <c r="J11" s="15"/>
+      <c r="J11" s="14" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="12" spans="4:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="13">
+      <c r="E12" s="22">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="F12" s="13">
+      <c r="F12" s="22">
         <v>6</v>
       </c>
-      <c r="G12" s="13">
+      <c r="G12" s="22">
         <v>7</v>
       </c>
-      <c r="H12" s="13">
+      <c r="H12" s="22">
         <v>9</v>
       </c>
-      <c r="I12" s="14">
+      <c r="I12" s="23">
         <v>28</v>
       </c>
-      <c r="J12" s="15"/>
+      <c r="J12" s="24" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="13" spans="4:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D13" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="13">
+      <c r="E13" s="12">
         <v>5.1999999999999998E-2</v>
       </c>
-      <c r="F13" s="13">
+      <c r="F13" s="12">
         <v>6</v>
       </c>
-      <c r="G13" s="13">
+      <c r="G13" s="12">
         <v>55</v>
       </c>
-      <c r="H13" s="13">
+      <c r="H13" s="12">
         <v>57</v>
       </c>
-      <c r="I13" s="14">
+      <c r="I13" s="13">
         <v>224</v>
       </c>
-      <c r="J13" s="15"/>
+      <c r="J13" s="14" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="14" spans="4:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D14" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="13">
+      <c r="E14" s="12">
         <v>6.0999999999999999E-2</v>
       </c>
-      <c r="F14" s="13">
+      <c r="F14" s="12">
         <v>6</v>
       </c>
-      <c r="G14" s="13">
+      <c r="G14" s="12">
         <v>41</v>
       </c>
-      <c r="H14" s="13">
+      <c r="H14" s="12">
         <v>43</v>
       </c>
-      <c r="I14" s="14">
+      <c r="I14" s="13">
         <v>170</v>
       </c>
-      <c r="J14" s="15"/>
+      <c r="J14" s="14" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="15" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D15" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="19">
+      <c r="E15" s="18">
         <v>0.874</v>
       </c>
-      <c r="F15" s="20">
+      <c r="F15" s="19">
         <v>6</v>
       </c>
-      <c r="G15" s="16">
+      <c r="G15" s="15">
         <v>11</v>
       </c>
-      <c r="H15" s="16">
+      <c r="H15" s="15">
         <v>13</v>
       </c>
-      <c r="I15" s="17">
+      <c r="I15" s="16">
         <v>50</v>
       </c>
-      <c r="J15" s="18"/>
+      <c r="J15" s="17" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="19" spans="4:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D19" s="1" t="s">
@@ -976,26 +1059,26 @@
       </c>
     </row>
     <row r="20" spans="4:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D21" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="E21" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G21" s="7" t="s">
+      <c r="G21" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H21" s="7" t="s">
+      <c r="H21" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I21" s="8" t="s">
+      <c r="I21" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J21" s="21" t="s">
+      <c r="J21" s="20" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1003,111 +1086,231 @@
       <c r="D22" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="12"/>
+      <c r="E22" s="12">
+        <v>40.392000000000003</v>
+      </c>
+      <c r="F22" s="12">
+        <v>9</v>
+      </c>
+      <c r="G22" s="12">
+        <v>3343</v>
+      </c>
+      <c r="H22" s="12">
+        <v>4609</v>
+      </c>
+      <c r="I22" s="12">
+        <v>30509</v>
+      </c>
+      <c r="J22" s="14" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="23" spans="4:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="15"/>
+      <c r="E23" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="F23" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="G23" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="H23" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="I23" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="J23" s="27" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="24" spans="4:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D24" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="15"/>
+      <c r="E24" s="12">
+        <v>4.2569999999999997</v>
+      </c>
+      <c r="F24" s="12">
+        <v>619</v>
+      </c>
+      <c r="G24" s="12">
+        <v>624</v>
+      </c>
+      <c r="H24" s="12">
+        <v>625</v>
+      </c>
+      <c r="I24" s="12">
+        <v>5602</v>
+      </c>
+      <c r="J24" s="14" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="25" spans="4:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="15"/>
+      <c r="E25" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="F25" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="G25" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="H25" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="I25" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="J25" s="30" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="26" spans="4:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D26" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="14"/>
-      <c r="J26" s="15"/>
+      <c r="E26" s="12">
+        <v>14.981</v>
+      </c>
+      <c r="F26" s="12">
+        <v>9</v>
+      </c>
+      <c r="G26" s="12">
+        <v>4849</v>
+      </c>
+      <c r="H26" s="12">
+        <v>4851</v>
+      </c>
+      <c r="I26" s="12">
+        <v>44001</v>
+      </c>
+      <c r="J26" s="14" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="27" spans="4:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="14"/>
-      <c r="J27" s="15"/>
+      <c r="E27" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="F27" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="G27" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="H27" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="I27" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="J27" s="30" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="28" spans="4:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="D28" s="5" t="s">
+      <c r="D28" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="13"/>
-      <c r="I28" s="14"/>
-      <c r="J28" s="15"/>
+      <c r="E28" s="22">
+        <v>2.3580000000000001</v>
+      </c>
+      <c r="F28" s="22">
+        <v>16</v>
+      </c>
+      <c r="G28" s="22">
+        <v>966</v>
+      </c>
+      <c r="H28" s="22">
+        <v>968</v>
+      </c>
+      <c r="I28" s="22">
+        <v>8694</v>
+      </c>
+      <c r="J28" s="24" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="29" spans="4:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D29" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
-      <c r="I29" s="14"/>
-      <c r="J29" s="15"/>
+      <c r="E29" s="12">
+        <v>11.917</v>
+      </c>
+      <c r="F29" s="12">
+        <v>9</v>
+      </c>
+      <c r="G29" s="12">
+        <v>4849</v>
+      </c>
+      <c r="H29" s="12">
+        <v>4851</v>
+      </c>
+      <c r="I29" s="12">
+        <v>44001</v>
+      </c>
+      <c r="J29" s="14" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="30" spans="4:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D30" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
-      <c r="I30" s="14"/>
-      <c r="J30" s="15"/>
+      <c r="E30" s="12">
+        <v>4.2389999999999999</v>
+      </c>
+      <c r="F30" s="12">
+        <v>9</v>
+      </c>
+      <c r="G30" s="12">
+        <v>1443</v>
+      </c>
+      <c r="H30" s="12">
+        <v>1445</v>
+      </c>
+      <c r="I30" s="12">
+        <v>13234</v>
+      </c>
+      <c r="J30" s="14" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="31" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D31" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E31" s="19"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="16"/>
-      <c r="H31" s="16"/>
-      <c r="I31" s="17"/>
-      <c r="J31" s="18"/>
+      <c r="E31" s="18">
+        <v>48.441000000000003</v>
+      </c>
+      <c r="F31" s="15">
+        <v>9</v>
+      </c>
+      <c r="G31" s="19">
+        <v>85</v>
+      </c>
+      <c r="H31" s="15">
+        <v>87</v>
+      </c>
+      <c r="I31" s="19">
+        <v>831</v>
+      </c>
+      <c r="J31" s="17" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="36" spans="4:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D36" s="1" t="s">
@@ -1115,26 +1318,26 @@
       </c>
     </row>
     <row r="37" spans="4:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="38" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D38" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E38" s="7" t="s">
+      <c r="E38" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F38" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G38" s="7" t="s">
+      <c r="G38" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H38" s="7" t="s">
+      <c r="H38" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I38" s="8" t="s">
+      <c r="I38" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="J38" s="21" t="s">
+      <c r="J38" s="20" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1142,111 +1345,111 @@
       <c r="D39" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E39" s="9"/>
-      <c r="F39" s="9"/>
-      <c r="G39" s="9"/>
-      <c r="H39" s="10"/>
-      <c r="I39" s="11"/>
-      <c r="J39" s="12"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="9"/>
+      <c r="I39" s="10"/>
+      <c r="J39" s="11"/>
     </row>
     <row r="40" spans="4:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D40" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E40" s="13"/>
-      <c r="F40" s="13"/>
-      <c r="G40" s="13"/>
-      <c r="H40" s="13"/>
-      <c r="I40" s="14"/>
-      <c r="J40" s="15"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="12"/>
+      <c r="H40" s="12"/>
+      <c r="I40" s="13"/>
+      <c r="J40" s="14"/>
     </row>
     <row r="41" spans="4:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D41" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E41" s="13"/>
-      <c r="F41" s="13"/>
-      <c r="G41" s="13"/>
-      <c r="H41" s="13"/>
-      <c r="I41" s="14"/>
-      <c r="J41" s="15"/>
+      <c r="E41" s="12"/>
+      <c r="F41" s="12"/>
+      <c r="G41" s="12"/>
+      <c r="H41" s="12"/>
+      <c r="I41" s="13"/>
+      <c r="J41" s="14"/>
     </row>
     <row r="42" spans="4:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D42" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E42" s="13"/>
-      <c r="F42" s="13"/>
-      <c r="G42" s="13"/>
-      <c r="H42" s="13"/>
-      <c r="I42" s="14"/>
-      <c r="J42" s="15"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="12"/>
+      <c r="H42" s="12"/>
+      <c r="I42" s="13"/>
+      <c r="J42" s="14"/>
     </row>
     <row r="43" spans="4:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D43" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E43" s="13"/>
-      <c r="F43" s="13"/>
-      <c r="G43" s="13"/>
-      <c r="H43" s="13"/>
-      <c r="I43" s="14"/>
-      <c r="J43" s="15"/>
+      <c r="E43" s="12"/>
+      <c r="F43" s="12"/>
+      <c r="G43" s="12"/>
+      <c r="H43" s="12"/>
+      <c r="I43" s="13"/>
+      <c r="J43" s="14"/>
     </row>
     <row r="44" spans="4:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D44" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E44" s="13"/>
-      <c r="F44" s="13"/>
-      <c r="G44" s="13"/>
-      <c r="H44" s="13"/>
-      <c r="I44" s="14"/>
-      <c r="J44" s="15"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="12"/>
+      <c r="G44" s="12"/>
+      <c r="H44" s="12"/>
+      <c r="I44" s="13"/>
+      <c r="J44" s="14"/>
     </row>
     <row r="45" spans="4:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D45" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E45" s="13"/>
-      <c r="F45" s="13"/>
-      <c r="G45" s="13"/>
-      <c r="H45" s="13"/>
-      <c r="I45" s="14"/>
-      <c r="J45" s="15"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="12"/>
+      <c r="H45" s="12"/>
+      <c r="I45" s="13"/>
+      <c r="J45" s="14"/>
     </row>
     <row r="46" spans="4:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D46" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E46" s="13"/>
-      <c r="F46" s="13"/>
-      <c r="G46" s="13"/>
-      <c r="H46" s="13"/>
-      <c r="I46" s="14"/>
-      <c r="J46" s="15"/>
+      <c r="E46" s="12"/>
+      <c r="F46" s="12"/>
+      <c r="G46" s="12"/>
+      <c r="H46" s="12"/>
+      <c r="I46" s="13"/>
+      <c r="J46" s="14"/>
     </row>
     <row r="47" spans="4:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D47" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E47" s="13"/>
-      <c r="F47" s="13"/>
-      <c r="G47" s="13"/>
-      <c r="H47" s="13"/>
-      <c r="I47" s="14"/>
-      <c r="J47" s="15"/>
+      <c r="E47" s="12"/>
+      <c r="F47" s="12"/>
+      <c r="G47" s="12"/>
+      <c r="H47" s="12"/>
+      <c r="I47" s="13"/>
+      <c r="J47" s="14"/>
     </row>
     <row r="48" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D48" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E48" s="19"/>
-      <c r="F48" s="20"/>
-      <c r="G48" s="16"/>
-      <c r="H48" s="16"/>
-      <c r="I48" s="17"/>
-      <c r="J48" s="18"/>
+      <c r="E48" s="18"/>
+      <c r="F48" s="19"/>
+      <c r="G48" s="15"/>
+      <c r="H48" s="15"/>
+      <c r="I48" s="16"/>
+      <c r="J48" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
bug: Spacing issue fixed
</commit_message>
<xml_diff>
--- a/Table for heuristics analysis.xlsx
+++ b/Table for heuristics analysis.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="27">
   <si>
     <t>Solving Air Cargo Problem 1</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>A*Search with h_1</t>
+  </si>
+  <si>
+    <t>A* Search with h_1</t>
   </si>
 </sst>
 </file>
@@ -933,8 +936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1155,7 +1158,7 @@
         <v>24</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E13" s="32">
         <v>5.1999999999999998E-2</v>

</xml_diff>

<commit_message>
feat: Problem 3 analysis
</commit_message>
<xml_diff>
--- a/Table for heuristics analysis.xlsx
+++ b/Table for heuristics analysis.xlsx
@@ -923,13 +923,13 @@
   <dimension ref="C3:J48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.85546875" customWidth="1"/>
     <col min="5" max="6" width="13.85546875" customWidth="1"/>
     <col min="7" max="7" width="15.7109375" customWidth="1"/>
     <col min="8" max="8" width="11.28515625" customWidth="1"/>
@@ -1696,7 +1696,7 @@
         <v>24</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E46" s="12">
         <v>53.786999999999999</v>
@@ -1741,9 +1741,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="48" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C48" s="45"/>
-      <c r="D48" s="25" t="s">
+      <c r="D48" s="39" t="s">
         <v>13</v>
       </c>
       <c r="E48" s="35" t="s">

</xml_diff>